<commit_message>
Massive update before I walk the dog
</commit_message>
<xml_diff>
--- a/Complaint-Data-Specifications.xlsx
+++ b/Complaint-Data-Specifications.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craig\source\repos\civilfiling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB07D537-2DB0-4DDF-A568-3001ED2C6D60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367447CC-FF79-4057-B7AD-DE1EADB0EE53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13642" yWindow="1747" windowWidth="17191" windowHeight="13081" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="1913" windowWidth="23460" windowHeight="13837" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSample-Pivot" sheetId="3" r:id="rId1"/>
@@ -101,9 +101,6 @@
     <t>Max 30 chars</t>
   </si>
   <si>
-    <t>9 digit numeric</t>
-  </si>
-  <si>
     <t>Less than 15000 and accepts up to two decimal places</t>
   </si>
   <si>
@@ -441,6 +438,9 @@
   </si>
   <si>
     <t>Max 30 Characters, CorporationName</t>
+  </si>
+  <si>
+    <t>9 digit numeric - Must be 9 digits</t>
   </si>
 </sst>
 </file>
@@ -973,7 +973,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
@@ -995,7 +995,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
@@ -1006,7 +1006,7 @@
         <v>6</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
@@ -1017,7 +1017,7 @@
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
@@ -1028,7 +1028,7 @@
         <v>8</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
@@ -1039,7 +1039,7 @@
         <v>9</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
@@ -1050,7 +1050,7 @@
         <v>10</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
@@ -1058,7 +1058,7 @@
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>22</v>
@@ -1069,23 +1069,23 @@
         <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
@@ -1093,7 +1093,7 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
@@ -1101,18 +1101,18 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
@@ -1120,10 +1120,10 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
@@ -1131,7 +1131,7 @@
         <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
@@ -1139,40 +1139,40 @@
         <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.45">
@@ -1180,10 +1180,10 @@
         <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.45">
@@ -1191,7 +1191,7 @@
         <v>21</v>
       </c>
       <c r="B30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.45">
@@ -1199,10 +1199,10 @@
         <v>20</v>
       </c>
       <c r="B31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
@@ -1210,10 +1210,10 @@
         <v>20</v>
       </c>
       <c r="B32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.45">
@@ -1221,10 +1221,10 @@
         <v>20</v>
       </c>
       <c r="B33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.45">
@@ -1232,7 +1232,7 @@
         <v>21</v>
       </c>
       <c r="B34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.45">
@@ -1240,19 +1240,19 @@
         <v>21</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C35" s="16"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.45">
@@ -1260,7 +1260,7 @@
         <v>20</v>
       </c>
       <c r="B37" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>22</v>
@@ -1271,26 +1271,26 @@
         <v>21</v>
       </c>
       <c r="B38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A40" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B40" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.45">
@@ -1298,40 +1298,40 @@
         <v>21</v>
       </c>
       <c r="B41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A42" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B44" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.45">
@@ -1339,10 +1339,10 @@
         <v>21</v>
       </c>
       <c r="B45" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.45">
@@ -1350,7 +1350,7 @@
         <v>21</v>
       </c>
       <c r="B46" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.45">
@@ -1358,10 +1358,10 @@
         <v>21</v>
       </c>
       <c r="B47" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.45">
@@ -1369,10 +1369,10 @@
         <v>21</v>
       </c>
       <c r="B48" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.45">
@@ -1380,7 +1380,7 @@
         <v>21</v>
       </c>
       <c r="B49" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C49" s="1">
         <v>7054</v>
@@ -1391,7 +1391,7 @@
         <v>21</v>
       </c>
       <c r="B50" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.45">
@@ -1399,38 +1399,38 @@
         <v>21</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E51" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B52" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C52" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="E52" t="s">
         <v>49</v>
-      </c>
-      <c r="B52" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="C52" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="E52" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B53" t="s">
+        <v>90</v>
+      </c>
+      <c r="C53" s="11" t="s">
         <v>91</v>
-      </c>
-      <c r="C53" s="11" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.45">
@@ -1438,7 +1438,7 @@
         <v>21</v>
       </c>
       <c r="B54" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C54" s="1">
         <v>0</v>
@@ -1446,21 +1446,21 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B55" t="s">
+        <v>94</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="B55" t="s">
-        <v>95</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B56" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C56" s="1">
         <v>999000111</v>
@@ -1471,7 +1471,7 @@
         <v>21</v>
       </c>
       <c r="B57" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C57" s="1">
         <v>1</v>
@@ -1482,18 +1482,18 @@
         <v>20</v>
       </c>
       <c r="B58" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A59" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B59" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1506,8 +1506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1529,7 +1529,7 @@
         <v>19</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
@@ -1543,7 +1543,7 @@
         <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
@@ -1557,7 +1557,7 @@
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.45">
@@ -1571,7 +1571,7 @@
         <v>20</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.45">
@@ -1599,7 +1599,7 @@
         <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
@@ -1621,13 +1621,13 @@
         <v>3</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
@@ -1641,7 +1641,7 @@
         <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
@@ -1649,13 +1649,13 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
@@ -1663,13 +1663,13 @@
         <v>6</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
@@ -1677,13 +1677,13 @@
         <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
@@ -1691,13 +1691,13 @@
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
@@ -1705,13 +1705,13 @@
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.45">
@@ -1719,18 +1719,18 @@
         <v>10</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C15" s="25" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A16" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>22</v>
@@ -1739,37 +1739,37 @@
         <v>20</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D19" t="s">
         <v>23</v>
@@ -1777,226 +1777,226 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
+        <v>112</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>114</v>
-      </c>
       <c r="D22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A25" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B25" s="24"/>
       <c r="C25" s="25" t="s">
         <v>21</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A26" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A28" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B28" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="25" t="s">
-        <v>41</v>
-      </c>
       <c r="D28" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A29" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C29" s="19" t="s">
         <v>20</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A35" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B35" s="21"/>
       <c r="C35" s="22" t="s">
         <v>21</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C36" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D36" s="15" t="s">
         <v>49</v>
-      </c>
-      <c r="D36" s="15" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A37" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B37" s="18" t="s">
         <v>22</v>
@@ -2005,154 +2005,154 @@
         <v>20</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D38" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D39" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D40" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A42" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D42" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D43" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D44" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A45" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C45" s="19" t="s">
         <v>21</v>
       </c>
       <c r="D45" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D46" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D47" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D48" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B49" s="1">
         <v>7054</v>
@@ -2161,63 +2161,63 @@
         <v>21</v>
       </c>
       <c r="D49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D50" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A51" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B51" s="21"/>
       <c r="C51" s="22" t="s">
         <v>21</v>
       </c>
       <c r="D51" s="20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C52" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D52" s="15" t="s">
         <v>49</v>
-      </c>
-      <c r="D52" s="15" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A53" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B53" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="B53" s="17" t="s">
+      <c r="C53" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D53" s="17" t="s">
         <v>92</v>
-      </c>
-      <c r="C53" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="D53" s="17" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="54" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A54" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B54" s="18">
         <v>0</v>
@@ -2226,40 +2226,40 @@
         <v>21</v>
       </c>
       <c r="D54" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C55" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D55" t="s">
         <v>102</v>
-      </c>
-      <c r="D55" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B56" s="1">
         <v>999000111</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D56" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B57" s="1">
         <v>1</v>
@@ -2268,32 +2268,32 @@
         <v>21</v>
       </c>
       <c r="D57" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D58" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
+        <v>98</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C59" s="2" t="s">
-        <v>100</v>
-      </c>
       <c r="D59" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -2314,17 +2314,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to log data issues
</commit_message>
<xml_diff>
--- a/Complaint-Data-Specifications.xlsx
+++ b/Complaint-Data-Specifications.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craig\source\repos\civilfiling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367447CC-FF79-4057-B7AD-DE1EADB0EE53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF6A872-9590-48BA-9792-4A1BBB18CF1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1913" windowWidth="23460" windowHeight="13837" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2678" yWindow="735" windowWidth="23459" windowHeight="13838" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSample-Pivot" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="139">
   <si>
     <t>CourtSection</t>
   </si>
@@ -398,18 +398,12 @@
     <t>Refer to Language worksheet in Code Tables spreedsheet</t>
   </si>
   <si>
-    <t>Branch id of the firm the case if filed from</t>
-  </si>
-  <si>
     <t>3 digit numeric, Refer to the Case Action worksheet in the Code Tables spreadsheet</t>
   </si>
   <si>
     <t>3 letter venue code. Refer to the County worksheet in the Code Tables spreadsheet</t>
   </si>
   <si>
-    <t>Refer to ServiceMethod worksheet in Code Tables spreadsheet (not found). Used what I found in other xml files.</t>
-  </si>
-  <si>
     <t>Refer to the Party Affiliation worksheet in the Code Tables spreadsheet</t>
   </si>
   <si>
@@ -441,6 +435,15 @@
   </si>
   <si>
     <t>9 digit numeric - Must be 9 digits</t>
+  </si>
+  <si>
+    <t>0001</t>
+  </si>
+  <si>
+    <t>Branch id of the firm the case if filed from, 4 chars required, typically 0001</t>
+  </si>
+  <si>
+    <t>Refer to ServiceMethod worksheet in Code Tables spreadsheet (not found). Used what I found in other xml files. Must be 2 Chars.</t>
   </si>
 </sst>
 </file>
@@ -878,7 +881,7 @@
   <dimension ref="A1:E59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -928,8 +931,8 @@
       <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="8">
-        <v>1</v>
+      <c r="C4" s="9" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
@@ -1402,10 +1405,10 @@
         <v>87</v>
       </c>
       <c r="C51" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="E51" t="s">
         <v>132</v>
-      </c>
-      <c r="E51" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.45">
@@ -1416,7 +1419,7 @@
         <v>88</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E52" t="s">
         <v>49</v>
@@ -1506,8 +1509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1543,7 +1546,7 @@
         <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
@@ -1557,21 +1560,21 @@
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="24">
-        <v>1</v>
+      <c r="B4" s="4" t="s">
+        <v>136</v>
       </c>
       <c r="C4" s="25" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.45">
@@ -1599,7 +1602,7 @@
         <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
@@ -1627,7 +1630,7 @@
         <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
@@ -1669,7 +1672,7 @@
         <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
@@ -1697,7 +1700,7 @@
         <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
@@ -1750,7 +1753,7 @@
         <v>21</v>
       </c>
       <c r="D17" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
@@ -1833,7 +1836,7 @@
         <v>21</v>
       </c>
       <c r="D24" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.45">
@@ -2024,13 +2027,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D39" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.45">
@@ -2041,7 +2044,7 @@
         <v>41</v>
       </c>
       <c r="D40" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.45">
@@ -2293,7 +2296,7 @@
         <v>99</v>
       </c>
       <c r="D59" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2324,7 +2327,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>